<commit_message>
Se modificó Doc Principal cap 2
</commit_message>
<xml_diff>
--- a/Planilla de horarios.xlsx
+++ b/Planilla de horarios.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pc\Documents\GitHub\RestApp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
@@ -82,11 +87,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -96,6 +102,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -144,7 +153,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -179,7 +188,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -388,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,6 +424,17 @@
         <v>3</v>
       </c>
       <c r="C2" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>41599</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
         <v>3</v>
       </c>
     </row>

</xml_diff>